<commit_message>
added data to query by,query added date, query assigned to
</commit_message>
<xml_diff>
--- a/Query_Log.xlsx
+++ b/Query_Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00 ASHOK IT\6AM\Project Tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVA Developer\Downloads\AshokITGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>SNO</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>How many contacts to display when we choose View all Contacts</t>
+  </si>
+  <si>
+    <t>C Madhu</t>
+  </si>
+  <si>
+    <t>Ashok</t>
   </si>
 </sst>
 </file>
@@ -140,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,6 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +442,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -447,10 +454,10 @@
     <col min="5" max="5" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -504,10 +511,16 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5">
+        <v>44008</v>
+      </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -522,10 +535,16 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44008</v>
+      </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -540,10 +559,16 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44008</v>
+      </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -558,10 +583,16 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="5">
+        <v>44008</v>
+      </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>